<commit_message>
Temporary commit with fixed errors and new data in files
</commit_message>
<xml_diff>
--- a/uvispace/uvisensor/datatemp/masterfile.xlsx
+++ b/uvispace/uvisensor/datatemp/masterfile.xlsx
@@ -391,7 +391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C20" activeCellId="0" pane="topLeft" sqref="C20"/>
@@ -655,6 +655,105 @@
         <v>12742</v>
       </c>
     </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="n">
+        <v>16879.14</v>
+      </c>
+      <c r="B24" t="n">
+        <v>255</v>
+      </c>
+      <c r="C24" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="n">
+        <v>-42.235</v>
+      </c>
+      <c r="B25" t="n">
+        <v>9</v>
+      </c>
+      <c r="C25" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="n">
+        <v>-10.57</v>
+      </c>
+      <c r="B26" t="n">
+        <v>9</v>
+      </c>
+      <c r="C26" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="n">
+        <v>57.229</v>
+      </c>
+      <c r="B27" t="n">
+        <v>9</v>
+      </c>
+      <c r="C27" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>9</v>
+      </c>
+      <c r="C28" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="B29" t="n">
+        <v>9</v>
+      </c>
+      <c r="C29" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="n">
+        <v>116.591</v>
+      </c>
+      <c r="B30" t="n">
+        <v>9</v>
+      </c>
+      <c r="C30" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="n">
+        <v>-198409.563</v>
+      </c>
+      <c r="B31" t="n">
+        <v>9</v>
+      </c>
+      <c r="C31" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="n">
+        <v>129.059</v>
+      </c>
+      <c r="B32" t="n">
+        <v>9</v>
+      </c>
+      <c r="C32" t="n">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
New tests with the UGV
</commit_message>
<xml_diff>
--- a/uvispace/uvisensor/datatemp/masterfile.xlsx
+++ b/uvispace/uvisensor/datatemp/masterfile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Spd Lin</t>
   </si>
@@ -31,49 +31,51 @@
     <t>Filename</t>
   </si>
   <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>26_05_2017_1146</t>
+  </si>
+  <si>
+    <t>26_05_2017_1149</t>
+  </si>
+  <si>
+    <t>26_05_2017_1156</t>
+  </si>
+  <si>
+    <t>26_05_2017_1157</t>
+  </si>
+  <si>
+    <t>26_05_2017_1202</t>
+  </si>
+  <si>
+    <t>26_05_2017_1206</t>
+  </si>
+  <si>
+    <t>26_05_2017_1207</t>
+  </si>
+  <si>
+    <t>26_05_2017_1221</t>
+  </si>
+  <si>
+    <t>26_05_2017_1223</t>
+  </si>
+  <si>
+    <t>26_05_2017_1224</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>26_05_2017_0945</t>
-  </si>
-  <si>
-    <t>26_05_2017_0957</t>
-  </si>
-  <si>
-    <t>26_05_2017_1009</t>
-  </si>
-  <si>
-    <t>26_05_2017_1013</t>
-  </si>
-  <si>
-    <t>26_05_2017_1015</t>
-  </si>
-  <si>
-    <t>26_05_2017_1017</t>
-  </si>
-  <si>
-    <t>26_05_2017_1027</t>
-  </si>
-  <si>
-    <t>26_05_2017_1049</t>
-  </si>
-  <si>
-    <t>26_05_2017_1101</t>
-  </si>
-  <si>
-    <t>26_05_2017_1107</t>
-  </si>
-  <si>
-    <t>26_05_2017_1122</t>
+    <t>26_05_2017_1225</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.00" numFmtId="165"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -124,14 +126,11 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -441,19 +440,19 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E1" activeCellId="0" pane="topLeft" sqref="E1"/>
+      <selection activeCell="F2" activeCellId="0" pane="topLeft" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1025" min="1" style="1" width="10"/>
-    <col customWidth="1" max="2" min="2" style="3" width="10"/>
-    <col customWidth="1" max="3" min="3" style="3" width="10"/>
-    <col customWidth="1" max="4" min="4" style="3" width="15"/>
-    <col customWidth="1" max="5" min="5" style="3" width="15"/>
+    <col customWidth="1" max="2" min="2" style="2" width="10"/>
+    <col customWidth="1" max="3" min="3" style="2" width="10"/>
+    <col customWidth="1" max="4" min="4" style="2" width="15"/>
+    <col customWidth="1" max="5" min="5" style="2" width="15"/>
   </cols>
   <sheetData>
-    <row customHeight="1" s="3" r="1" ht="13.8" spans="1:5">
+    <row customHeight="1" s="2" r="1" ht="13.8" spans="1:5">
       <c s="1" r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,193 +469,195 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" s="3" r="2" ht="15" spans="1:5">
-      <c s="2" r="A2" t="n">
-        <v>-262.147460938</v>
-      </c>
-      <c s="2" r="B2" t="n">
-        <v>-14.5081605911</v>
-      </c>
-      <c s="2" r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c s="2" r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c s="2" r="E2" t="s">
+    <row customHeight="1" s="2" r="2" ht="15" spans="1:5">
+      <c s="3" r="A2" t="n">
+        <v>-12172.8818359</v>
+      </c>
+      <c s="3" r="B2" t="n">
+        <v>27.9913272858</v>
+      </c>
+      <c s="3" r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="E2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c s="4" r="A3" t="n">
-        <v>2.46675872803</v>
-      </c>
-      <c s="4" r="B3" t="n">
-        <v>-0.0201388597488</v>
-      </c>
-      <c s="4" r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="E3" t="s">
+    <row customHeight="1" s="2" r="3" ht="13.8" spans="1:5">
+      <c s="3" r="A3" t="n">
+        <v>28035.8457031</v>
+      </c>
+      <c s="3" r="B3" t="n">
+        <v>27.4060611725</v>
+      </c>
+      <c s="3" r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="E3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c s="4" r="A4" t="n">
-        <v>-162.789794922</v>
-      </c>
-      <c s="4" r="B4" t="n">
-        <v>0.0615426301956</v>
-      </c>
-      <c s="4" r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="E4" t="s">
+    <row customHeight="1" s="2" r="4" ht="13.8" spans="1:5">
+      <c s="3" r="A4" t="n">
+        <v>13430.0166016</v>
+      </c>
+      <c s="3" r="B4" t="n">
+        <v>-64.4532089233</v>
+      </c>
+      <c s="3" r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="E4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c s="4" r="A5" t="n">
-        <v>-26385.9042969</v>
-      </c>
-      <c s="4" r="B5" t="n">
-        <v>-12.059630394</v>
-      </c>
-      <c s="4" r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="E5" t="s">
+    <row customHeight="1" s="2" r="5" ht="13.8" spans="1:5">
+      <c s="3" r="A5" t="n">
+        <v>-17425.078125</v>
+      </c>
+      <c s="3" r="B5" t="n">
+        <v>0.392636060715</v>
+      </c>
+      <c s="3" r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="E5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c s="4" r="A6" t="n">
-        <v>1109.91467285</v>
-      </c>
-      <c s="4" r="B6" t="n">
-        <v>-1.18221211433</v>
-      </c>
-      <c s="4" r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="E6" t="s">
+    <row customHeight="1" s="2" r="6" ht="13.8" spans="1:5">
+      <c s="3" r="A6" t="n">
+        <v>19537.421875</v>
+      </c>
+      <c s="3" r="B6" t="n">
+        <v>-92.9751739502</v>
+      </c>
+      <c s="3" r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="E6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c s="4" r="A7" t="n">
-        <v>-2180.96118164</v>
-      </c>
-      <c s="4" r="B7" t="n">
-        <v>21.9433498383</v>
-      </c>
-      <c s="4" r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="E7" t="s">
+    <row customHeight="1" s="2" r="7" ht="13.8" spans="1:5">
+      <c s="3" r="A7" t="n">
+        <v>-16257.3505859</v>
+      </c>
+      <c s="3" r="B7" t="n">
+        <v>183.44291687</v>
+      </c>
+      <c s="3" r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="E7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c s="4" r="A8" t="n">
-        <v>-43.735710144</v>
-      </c>
-      <c s="4" r="B8" t="n">
-        <v>-0.298575162888</v>
-      </c>
-      <c s="4" r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="E8" t="s">
+    <row customHeight="1" s="2" r="8" ht="13.8" spans="1:5">
+      <c s="3" r="A8" t="n">
+        <v>24476.0332031</v>
+      </c>
+      <c s="3" r="B8" t="n">
+        <v>3.17313098907</v>
+      </c>
+      <c s="3" r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="E8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c s="4" r="A9" t="n">
-        <v>-1446.48046875</v>
-      </c>
-      <c s="4" r="B9" t="n">
-        <v>17.9434680939</v>
-      </c>
-      <c s="4" r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="E9" t="s">
+    <row customHeight="1" s="2" r="9" ht="13.8" spans="1:5">
+      <c s="3" r="A9" t="n">
+        <v>27264.7675781</v>
+      </c>
+      <c s="3" r="B9" t="n">
+        <v>40.8537483215</v>
+      </c>
+      <c s="3" r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="E9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c s="4" r="A10" t="n">
-        <v>31709.4667969</v>
-      </c>
-      <c s="4" r="B10" t="n">
-        <v>-76.2270202637</v>
-      </c>
-      <c s="4" r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="E10" t="s">
+    <row customHeight="1" s="2" r="10" ht="13.8" spans="1:5">
+      <c s="3" r="A10" t="n">
+        <v>-4763.77392578</v>
+      </c>
+      <c s="3" r="B10" t="n">
+        <v>51.455619812</v>
+      </c>
+      <c s="3" r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="E10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c s="4" r="A11" t="n">
-        <v>-20.5845489502</v>
-      </c>
-      <c s="4" r="B11" t="n">
-        <v>-0.0118002891541</v>
-      </c>
-      <c s="4" r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="E11" t="s">
+    <row customHeight="1" s="2" r="11" ht="13.8" spans="1:5">
+      <c s="3" r="A11" t="n">
+        <v>-26889.0019531</v>
+      </c>
+      <c s="3" r="B11" t="n">
+        <v>287.476623535</v>
+      </c>
+      <c s="3" r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c s="3" r="E11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c s="4" r="A12" t="n">
-        <v>340.821777344</v>
-      </c>
-      <c s="4" r="B12" t="n">
-        <v>-1.41657829285</v>
-      </c>
-      <c s="4" r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c s="4" r="E12" t="s">
+    <row customHeight="1" s="2" r="12" ht="13.8" spans="1:5">
+      <c s="3" r="A12" t="n">
+        <v>-22495.7539062</v>
+      </c>
+      <c s="3" r="B12" t="n">
+        <v>4.99187326431</v>
+      </c>
+      <c s="3" r="C12" t="s">
         <v>16</v>
       </c>
-    </row>
+      <c s="3" r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c s="3" r="E12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row customHeight="1" s="2" r="13" ht="13.8" spans="1:5"/>
+    <row customHeight="1" s="2" r="14" ht="13.8" spans="1:5"/>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
New data results and modified multiplecamera
</commit_message>
<xml_diff>
--- a/uvispace/uvisensor/datatemp/masterfile.xlsx
+++ b/uvispace/uvisensor/datatemp/masterfile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>Spd Lin</t>
   </si>
@@ -65,6 +65,36 @@
   </si>
   <si>
     <t>26_05_2017_1122</t>
+  </si>
+  <si>
+    <t>26_05_2017_1302</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>26_05_2017_1304</t>
+  </si>
+  <si>
+    <t>26_05_2017_1318</t>
+  </si>
+  <si>
+    <t>26_05_2017_1319</t>
+  </si>
+  <si>
+    <t>26_05_2017_1321</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>26_05_2017_1322</t>
+  </si>
+  <si>
+    <t>26_05_2017_1323</t>
+  </si>
+  <si>
+    <t>26_05_2017_1324</t>
   </si>
 </sst>
 </file>
@@ -438,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E1" activeCellId="0" pane="topLeft" sqref="E1"/>
@@ -657,6 +687,142 @@
         <v>16</v>
       </c>
     </row>
+    <row r="13" spans="1:5">
+      <c s="4" r="A13" t="n">
+        <v>-1583.58</v>
+      </c>
+      <c s="4" r="B13" t="n">
+        <v>-98.08</v>
+      </c>
+      <c s="4" r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c s="4" r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c s="4" r="E13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c s="4" r="A14" t="n">
+        <v>24606.82</v>
+      </c>
+      <c s="4" r="B14" t="n">
+        <v>-41.52</v>
+      </c>
+      <c s="4" r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c s="4" r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c s="4" r="E14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c s="4" r="A15" t="n">
+        <v>14071.75</v>
+      </c>
+      <c s="4" r="B15" t="n">
+        <v>7.63</v>
+      </c>
+      <c s="4" r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c s="4" r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c s="4" r="E15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c s="4" r="A16" t="n">
+        <v>3954.1</v>
+      </c>
+      <c s="4" r="B16" t="n">
+        <v>-23.1</v>
+      </c>
+      <c s="4" r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c s="4" r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c s="4" r="E16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c s="4" r="A17" t="n">
+        <v>12999.59</v>
+      </c>
+      <c s="4" r="B17" t="n">
+        <v>-83.64</v>
+      </c>
+      <c s="4" r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c s="4" r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c s="4" r="E17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c s="4" r="A18" t="n">
+        <v>-380.76</v>
+      </c>
+      <c s="4" r="B18" t="n">
+        <v>15.63</v>
+      </c>
+      <c s="4" r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c s="4" r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c s="4" r="E18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c s="4" r="A19" t="n">
+        <v>23743.07</v>
+      </c>
+      <c s="4" r="B19" t="n">
+        <v>-69.39</v>
+      </c>
+      <c s="4" r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c s="4" r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c s="4" r="E19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c s="4" r="A20" t="n">
+        <v>28092.45</v>
+      </c>
+      <c s="4" r="B20" t="n">
+        <v>-21.95</v>
+      </c>
+      <c s="4" r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c s="4" r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c s="4" r="E20" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>

</xml_diff>